<commit_message>
added some examples for reference
</commit_message>
<xml_diff>
--- a/reference/Calculate tax lot interest income from daily interest accruals.xlsx
+++ b/reference/Calculate tax lot interest income from daily interest accruals.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://chinalifefranklinamc.sharepoint.com/sites/IT618/Shared Documents/General/20201205 Bond Yield IMA Calculation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="245" documentId="13_ncr:1_{D783A27B-3919-4BA5-A606-8D1B6B2A3DBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{65B5F815-045B-4821-8B43-14CF134DA492}"/>
+  <xr:revisionPtr revIDLastSave="470" documentId="13_ncr:1_{D783A27B-3919-4BA5-A606-8D1B6B2A3DBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DFE056DF-740F-4DF5-B788-507CE6214278}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{03EDCEC2-7A62-4842-A00E-4319C8C9FA05}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{03EDCEC2-7A62-4842-A00E-4319C8C9FA05}"/>
   </bookViews>
   <sheets>
     <sheet name="Observation" sheetId="1" r:id="rId1"/>
     <sheet name="tax lot coupon cash flow" sheetId="2" r:id="rId2"/>
+    <sheet name="examples" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="86">
   <si>
     <t>Interest Income</t>
   </si>
@@ -236,15 +237,73 @@
   </si>
   <si>
     <t>Calculate coupon cash flow per tax lot</t>
+  </si>
+  <si>
+    <t>GBHK 2.93 01/13/20</t>
+  </si>
+  <si>
+    <t>Matures on 2020-01-13</t>
+  </si>
+  <si>
+    <t>problem: last line on 2020-01-13 has accrued interest = 0</t>
+  </si>
+  <si>
+    <t>HKTB 0 04/29/20 91</t>
+  </si>
+  <si>
+    <t>Tax lot Id</t>
+  </si>
+  <si>
+    <t>Interest Income from P/L report</t>
+  </si>
+  <si>
+    <t>Zero coupon bond bought on 2020-02</t>
+  </si>
+  <si>
+    <t>problem: tax lot does not exist in daily interet accrual detail report at all</t>
+  </si>
+  <si>
+    <t>CNOOC 7.5 07/30/39</t>
+  </si>
+  <si>
+    <t>Has 4 tax lots on 2019-12-31, buys 2 more tax lots on 2020-01, pays interest on 2020-01-30</t>
+  </si>
+  <si>
+    <t>Tax lot id</t>
+  </si>
+  <si>
+    <t>Coupon Received</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Coupon</t>
+  </si>
+  <si>
+    <t>Total Interest Income</t>
+  </si>
+  <si>
+    <t>problem: when the tax lot was bought, it has accrued interest</t>
+  </si>
+  <si>
+    <t>Starting AI</t>
+  </si>
+  <si>
+    <t>Ending AI</t>
+  </si>
+  <si>
+    <t>Interet Bought</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -324,7 +383,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -361,6 +420,7 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -969,16 +1029,16 @@
       </c>
     </row>
     <row r="42" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="26" t="s">
+      <c r="A42" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B42" s="26"/>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26"/>
-      <c r="G42" s="26"/>
-      <c r="H42" s="26"/>
+      <c r="B42" s="27"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="27"/>
+      <c r="F42" s="27"/>
+      <c r="G42" s="27"/>
+      <c r="H42" s="27"/>
     </row>
     <row r="43" spans="1:8" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
@@ -1311,16 +1371,16 @@
       </c>
     </row>
     <row r="72" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="26" t="s">
+      <c r="A72" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B72" s="26"/>
-      <c r="C72" s="26"/>
-      <c r="D72" s="26"/>
-      <c r="E72" s="26"/>
-      <c r="F72" s="26"/>
-      <c r="G72" s="26"/>
-      <c r="H72" s="26"/>
+      <c r="B72" s="27"/>
+      <c r="C72" s="27"/>
+      <c r="D72" s="27"/>
+      <c r="E72" s="27"/>
+      <c r="F72" s="27"/>
+      <c r="G72" s="27"/>
+      <c r="H72" s="27"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
@@ -1476,8 +1536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDF58FBF-87C5-40DC-B96D-BBE031B8A272}">
   <dimension ref="A1:W44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2537,19 +2597,391 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5075E231-314A-4BC9-B246-6DF080AB1E4D}">
+  <dimension ref="A1:O23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.875" customWidth="1"/>
+    <col min="2" max="3" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.75" customWidth="1"/>
+    <col min="5" max="5" width="14.25" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="10" max="10" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.75" customWidth="1"/>
+    <col min="14" max="14" width="14.75" customWidth="1"/>
+    <col min="15" max="15" width="12.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1108340</v>
+      </c>
+      <c r="B3" s="16">
+        <v>679093.73</v>
+      </c>
+      <c r="C3" s="16">
+        <v>726198.49</v>
+      </c>
+      <c r="D3" s="20">
+        <f>C3-B3</f>
+        <v>47104.760000000009</v>
+      </c>
+      <c r="E3" s="16">
+        <v>47104.76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="20"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I13" t="s">
+        <v>79</v>
+      </c>
+      <c r="J13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1104216</v>
+      </c>
+      <c r="B14" s="16">
+        <v>1224594.27</v>
+      </c>
+      <c r="C14" s="16">
+        <v>8091.98</v>
+      </c>
+      <c r="D14" s="16">
+        <f>J15</f>
+        <v>1456237.5</v>
+      </c>
+      <c r="E14" s="16">
+        <f>C14-B14+D14</f>
+        <v>239735.20999999996</v>
+      </c>
+      <c r="I14" s="26">
+        <f>SUM(I15:I20)</f>
+        <v>31000000</v>
+      </c>
+      <c r="J14" s="16">
+        <v>9028672.5</v>
+      </c>
+      <c r="M14" t="s">
+        <v>43</v>
+      </c>
+      <c r="N14" t="s">
+        <v>44</v>
+      </c>
+      <c r="O14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1104217</v>
+      </c>
+      <c r="B15" s="16">
+        <v>1224594.27</v>
+      </c>
+      <c r="C15" s="16">
+        <v>8091.98</v>
+      </c>
+      <c r="D15" s="16">
+        <f t="shared" ref="D15:D19" si="0">J16</f>
+        <v>1456237.5</v>
+      </c>
+      <c r="E15" s="16">
+        <f t="shared" ref="E15:E19" si="1">C15-B15+D15</f>
+        <v>239735.20999999996</v>
+      </c>
+      <c r="F15" s="16"/>
+      <c r="H15">
+        <v>1104216</v>
+      </c>
+      <c r="I15" s="26">
+        <v>5000000</v>
+      </c>
+      <c r="J15" s="20">
+        <f>I15/$I$14*$J$14</f>
+        <v>1456237.5</v>
+      </c>
+      <c r="L15">
+        <v>1109831</v>
+      </c>
+      <c r="M15" s="16">
+        <v>8095.29</v>
+      </c>
+      <c r="N15" s="16">
+        <v>1327631.25</v>
+      </c>
+      <c r="O15" s="16">
+        <f>N15-M15</f>
+        <v>1319535.96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1104496</v>
+      </c>
+      <c r="B16" s="16">
+        <v>1224594.27</v>
+      </c>
+      <c r="C16" s="16">
+        <v>8091.98</v>
+      </c>
+      <c r="D16" s="16">
+        <f t="shared" si="0"/>
+        <v>1456237.5</v>
+      </c>
+      <c r="E16" s="16">
+        <f t="shared" si="1"/>
+        <v>239735.20999999996</v>
+      </c>
+      <c r="F16" s="16"/>
+      <c r="H16">
+        <v>1104217</v>
+      </c>
+      <c r="I16" s="26">
+        <v>5000000</v>
+      </c>
+      <c r="J16" s="20">
+        <f t="shared" ref="J16:J20" si="2">I16/$I$14*$J$14</f>
+        <v>1456237.5</v>
+      </c>
+      <c r="L16">
+        <v>1110346</v>
+      </c>
+      <c r="M16" s="16">
+        <v>16192.94</v>
+      </c>
+      <c r="N16" s="16">
+        <v>2704217.08</v>
+      </c>
+      <c r="O16" s="16">
+        <f>N16-M16</f>
+        <v>2688024.14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1104497</v>
+      </c>
+      <c r="B17" s="16">
+        <v>244918.85</v>
+      </c>
+      <c r="C17" s="16">
+        <v>1618.4</v>
+      </c>
+      <c r="D17" s="16">
+        <f t="shared" si="0"/>
+        <v>291247.5</v>
+      </c>
+      <c r="E17" s="16">
+        <f t="shared" si="1"/>
+        <v>47947.049999999988</v>
+      </c>
+      <c r="F17" s="16"/>
+      <c r="H17">
+        <v>1104496</v>
+      </c>
+      <c r="I17" s="26">
+        <v>5000000</v>
+      </c>
+      <c r="J17" s="20">
+        <f t="shared" si="2"/>
+        <v>1456237.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1109831</v>
+      </c>
+      <c r="B18" s="16">
+        <f>O15</f>
+        <v>1319535.96</v>
+      </c>
+      <c r="C18" s="16">
+        <v>8091.98</v>
+      </c>
+      <c r="D18" s="16">
+        <f t="shared" si="0"/>
+        <v>1456237.5</v>
+      </c>
+      <c r="E18" s="16">
+        <f t="shared" si="1"/>
+        <v>144793.52000000002</v>
+      </c>
+      <c r="F18" s="16"/>
+      <c r="H18">
+        <v>1104497</v>
+      </c>
+      <c r="I18" s="26">
+        <v>1000000</v>
+      </c>
+      <c r="J18" s="20">
+        <f t="shared" si="2"/>
+        <v>291247.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1110346</v>
+      </c>
+      <c r="B19" s="16">
+        <f>O16</f>
+        <v>2688024.14</v>
+      </c>
+      <c r="C19" s="16">
+        <v>16183.96</v>
+      </c>
+      <c r="D19" s="16">
+        <f t="shared" si="0"/>
+        <v>2912475</v>
+      </c>
+      <c r="E19" s="16">
+        <f t="shared" si="1"/>
+        <v>240634.81999999983</v>
+      </c>
+      <c r="H19">
+        <v>1109831</v>
+      </c>
+      <c r="I19" s="26">
+        <v>5000000</v>
+      </c>
+      <c r="J19" s="20">
+        <f t="shared" si="2"/>
+        <v>1456237.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="D20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" s="20">
+        <f>SUM(E14:E19)</f>
+        <v>1152581.0199999998</v>
+      </c>
+      <c r="H20">
+        <v>1110346</v>
+      </c>
+      <c r="I20" s="26">
+        <v>10000000</v>
+      </c>
+      <c r="J20" s="20">
+        <f t="shared" si="2"/>
+        <v>2912475</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="C21" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" s="16">
+        <v>1152581.02</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" s="20"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2731,18 +3163,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86950AF1-3B0F-4325-898D-5495113D013F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9D5D619-8B2D-4F02-88F7-AF4B83361BA6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9D5D619-8B2D-4F02-88F7-AF4B83361BA6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86950AF1-3B0F-4325-898D-5495113D013F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
updated excel examples a bit
</commit_message>
<xml_diff>
--- a/reference/Calculate tax lot interest income from daily interest accruals.xlsx
+++ b/reference/Calculate tax lot interest income from daily interest accruals.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steven.zhang\AppData\Local\Programs\Git\git\clamc_yield_report\reference\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhangst\git\clamc_yield_report\reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF7D12C-2F5D-4CA2-A725-35E885583E14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F626909-D5CE-4789-B599-0EDCB22A2C9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{03EDCEC2-7A62-4842-A00E-4319C8C9FA05}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{03EDCEC2-7A62-4842-A00E-4319C8C9FA05}"/>
   </bookViews>
   <sheets>
     <sheet name="examples" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="124">
   <si>
     <t>Interest Income</t>
   </si>
@@ -339,24 +339,15 @@
     <t>Reduction Process</t>
   </si>
   <si>
-    <t>1) remove a tax lot whose LotQuantity = 0 from the above table;</t>
-  </si>
-  <si>
     <t>Reduction Round 1: take out tax lot 1005791</t>
   </si>
   <si>
     <t>Reduction Round 2: take out tax lot 1005793</t>
   </si>
   <si>
-    <t>Here we have tax lots with LotQuantity = 0, and such tax lots does not receive interest payment at all. So we need to start the below reduction process to take them out.</t>
-  </si>
-  <si>
     <t>First of all, construct the below table with all tax lots (whether their quantity = 0 or not)</t>
   </si>
   <si>
-    <t>2) update the total Interest payment amount as: total interest payment = total interest payment + LotSumOfChangeInAIBook of the tax lot removed.</t>
-  </si>
-  <si>
     <t>When the table becomes empty, the process is over, no tax lot receives any interest income.</t>
   </si>
   <si>
@@ -393,13 +384,28 @@
     <t>V0 * z0 / S</t>
   </si>
   <si>
-    <t>When the table is left with tax lots whose quantity &gt; 0, such as below. Then we apply the pro-rata method to get interest income for remaining tax lots.</t>
-  </si>
-  <si>
     <t>Similarly, when we apply reduction process on tax lot 1108340, it does not get any interest income from the interest payment event.</t>
   </si>
   <si>
     <t>Total Interest Received</t>
+  </si>
+  <si>
+    <t>Special Case: Tax lots with LotQuantity = 0</t>
+  </si>
+  <si>
+    <t>When we have tax lots with LotQuantity = 0, we need to take them out before computing any interest received. Because tax lots whose quantity are zero do not receive any interests.</t>
+  </si>
+  <si>
+    <t>3) Go back to step 1 if there are still tax lots whose LotQuantity = 0.</t>
+  </si>
+  <si>
+    <t>1) Remove a tax lot whose LotQuantity = 0 from the above table;</t>
+  </si>
+  <si>
+    <t>2) Update the total Interest payment amount as: total interest payment = total interest payment + LotSumOfChangeInAIBook of the tax lot removed;</t>
+  </si>
+  <si>
+    <t>When the table is left with only tax lots whose quantity &gt; 0, such as below. Then we apply the pro-rata method to get interest income for remaining tax lots.</t>
   </si>
 </sst>
 </file>
@@ -410,7 +416,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -441,6 +447,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <i/>
       <sz val="12"/>
       <color theme="1"/>
@@ -494,7 +509,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -524,6 +539,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="43" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -536,8 +553,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -853,36 +869,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5075E231-314A-4BC9-B246-6DF080AB1E4D}">
-  <dimension ref="A1:X297"/>
+  <dimension ref="A1:X299"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A221" workbookViewId="0">
-      <selection activeCell="L210" sqref="L210"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E281" sqref="E281"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.375" customWidth="1"/>
-    <col min="2" max="2" width="13.75" customWidth="1"/>
-    <col min="3" max="3" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.75" customWidth="1"/>
-    <col min="5" max="5" width="15.875" customWidth="1"/>
-    <col min="6" max="6" width="12.875" customWidth="1"/>
-    <col min="7" max="7" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.875" customWidth="1"/>
+    <col min="1" max="1" width="9.3984375" customWidth="1"/>
+    <col min="2" max="2" width="13.69921875" customWidth="1"/>
+    <col min="3" max="3" width="15.09765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.69921875" customWidth="1"/>
+    <col min="5" max="5" width="15.8984375" customWidth="1"/>
+    <col min="6" max="6" width="12.8984375" customWidth="1"/>
+    <col min="7" max="7" width="11.09765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.8984375" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.75" customWidth="1"/>
-    <col min="14" max="14" width="14.75" customWidth="1"/>
-    <col min="15" max="15" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.69921875" customWidth="1"/>
+    <col min="14" max="14" width="14.69921875" customWidth="1"/>
+    <col min="15" max="15" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.8984375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.09765625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.09765625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.69921875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>74</v>
       </c>
@@ -892,12 +908,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>75</v>
       </c>
@@ -907,7 +923,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -925,7 +941,7 @@
       </c>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1104216</v>
       </c>
@@ -946,7 +962,7 @@
       <c r="I7" s="9"/>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1104217</v>
       </c>
@@ -971,7 +987,7 @@
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1104496</v>
       </c>
@@ -996,7 +1012,7 @@
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1104497</v>
       </c>
@@ -1018,7 +1034,7 @@
       <c r="I10" s="9"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1109831</v>
       </c>
@@ -1040,7 +1056,7 @@
       <c r="I11" s="9"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1110346</v>
       </c>
@@ -1061,7 +1077,7 @@
       <c r="I12" s="9"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="D13" t="s">
         <v>27</v>
@@ -1073,7 +1089,7 @@
       <c r="I13" s="9"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="C14" t="s">
         <v>24</v>
@@ -1082,22 +1098,22 @@
         <v>1152581.02</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -1165,7 +1181,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
         <v>20</v>
       </c>
@@ -1223,7 +1239,7 @@
       <c r="W21" s="12"/>
       <c r="X21" s="12"/>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1273,7 +1289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -1323,7 +1339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -1373,7 +1389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -1423,7 +1439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -1473,7 +1489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -1523,10 +1539,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="E28" s="8"/>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>70</v>
       </c>
@@ -1538,7 +1554,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -1549,7 +1565,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A31">
         <f>H22</f>
         <v>1104216</v>
@@ -1563,7 +1579,7 @@
         <v>1456237.5</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A32">
         <f t="shared" ref="A32:A36" si="2">H23</f>
         <v>1104217</v>
@@ -1577,7 +1593,7 @@
         <v>1456237.5</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <f t="shared" si="2"/>
         <v>1104496</v>
@@ -1591,7 +1607,7 @@
         <v>1456237.5</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <f t="shared" si="2"/>
         <v>1104497</v>
@@ -1605,7 +1621,7 @@
         <v>291247.5</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <f t="shared" si="2"/>
         <v>1109831</v>
@@ -1619,7 +1635,7 @@
         <v>1456237.5</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <f t="shared" si="2"/>
         <v>1110346</v>
@@ -1633,7 +1649,7 @@
         <v>2912475</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>53</v>
       </c>
@@ -1642,7 +1658,7 @@
         <v>31000000</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>77</v>
       </c>
@@ -1650,7 +1666,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>25</v>
       </c>
@@ -1667,7 +1683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>1006824</v>
       </c>
@@ -1686,7 +1702,7 @@
         <v>11530.440305555552</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>1006825</v>
       </c>
@@ -1705,7 +1721,7 @@
         <v>19217.390509259247</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>1006826</v>
       </c>
@@ -1724,7 +1740,7 @@
         <v>19217.390509259247</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>1008174</v>
       </c>
@@ -1743,7 +1759,7 @@
         <v>172956.5345833333</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>1008175</v>
       </c>
@@ -1762,7 +1778,7 @@
         <v>65339.131731481466</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>1008176</v>
       </c>
@@ -1781,7 +1797,7 @@
         <v>38434.781018518494</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>1008177</v>
       </c>
@@ -1800,7 +1816,7 @@
         <v>172956.5345833333</v>
       </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>1021956</v>
       </c>
@@ -1819,7 +1835,7 @@
         <v>3651304.5167592578</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B50" s="6"/>
       <c r="D50" t="s">
         <v>27</v>
@@ -1829,7 +1845,7 @@
         <v>4150956.7199999983</v>
       </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C51" t="s">
         <v>24</v>
       </c>
@@ -1837,22 +1853,22 @@
         <v>4150956.72</v>
       </c>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>1</v>
       </c>
@@ -1920,7 +1936,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>20</v>
       </c>
@@ -1970,7 +1986,7 @@
         <v>779.79</v>
       </c>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>20</v>
       </c>
@@ -2020,7 +2036,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>20</v>
       </c>
@@ -2070,7 +2086,7 @@
         <v>1299.6500000000001</v>
       </c>
     </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>20</v>
       </c>
@@ -2120,7 +2136,7 @@
         <v>11696.85</v>
       </c>
     </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>20</v>
       </c>
@@ -2170,7 +2186,7 @@
         <v>4418.8100000000004</v>
       </c>
     </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>20</v>
       </c>
@@ -2220,7 +2236,7 @@
         <v>2599.3000000000002</v>
       </c>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>20</v>
       </c>
@@ -2270,7 +2286,7 @@
         <v>11696.85</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>20</v>
       </c>
@@ -2320,7 +2336,7 @@
         <v>246933.5</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A66" s="12" t="s">
         <v>20</v>
       </c>
@@ -2376,7 +2392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A67" s="12" t="s">
         <v>20</v>
       </c>
@@ -2432,7 +2448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A68" s="12" t="s">
         <v>20</v>
       </c>
@@ -2488,7 +2504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>70</v>
       </c>
@@ -2500,7 +2516,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>52</v>
       </c>
@@ -2511,7 +2527,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>1006824</v>
       </c>
@@ -2524,7 +2540,7 @@
         <v>69401.310305555555</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>1006825</v>
       </c>
@@ -2537,7 +2553,7 @@
         <v>115668.85050925925</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>1006826</v>
       </c>
@@ -2550,7 +2566,7 @@
         <v>115668.85050925925</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>1008174</v>
       </c>
@@ -2563,7 +2579,7 @@
         <v>1041019.6545833333</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>1008175</v>
       </c>
@@ -2576,7 +2592,7 @@
         <v>393274.09173148143</v>
       </c>
     </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>1008176</v>
       </c>
@@ -2589,7 +2605,7 @@
         <v>231337.70101851851</v>
       </c>
     </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>1008177</v>
       </c>
@@ -2602,7 +2618,7 @@
         <v>1041019.6545833333</v>
       </c>
     </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>1021956</v>
       </c>
@@ -2615,7 +2631,7 @@
         <v>21977081.59675926</v>
       </c>
     </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>53</v>
       </c>
@@ -2624,7 +2640,7 @@
         <v>108000000</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>78</v>
       </c>
@@ -2634,7 +2650,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>25</v>
       </c>
@@ -2651,7 +2667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A85" s="5">
         <v>1115230</v>
       </c>
@@ -2671,7 +2687,7 @@
       </c>
       <c r="M85" s="6"/>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A86" s="5">
         <v>1115231</v>
       </c>
@@ -2690,7 +2706,7 @@
         <v>42323.237216859998</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A87" s="5">
         <v>1115402</v>
       </c>
@@ -2709,7 +2725,7 @@
         <v>1269697.06278314</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A88" s="5">
         <v>1115403</v>
       </c>
@@ -2728,7 +2744,7 @@
         <v>781119.09333333338</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A89" s="5">
         <v>1115431</v>
       </c>
@@ -2747,7 +2763,7 @@
         <v>87468.02</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>1118798</v>
       </c>
@@ -2766,7 +2782,7 @@
         <v>7025.1886666666669</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>1118799</v>
       </c>
@@ -2785,7 +2801,7 @@
         <v>7025.1886666666669</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>1118800</v>
       </c>
@@ -2807,7 +2823,7 @@
       <c r="O92" s="1"/>
       <c r="P92" s="8"/>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>1118801</v>
       </c>
@@ -2826,7 +2842,7 @@
         <v>7025.1886666666669</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>1118802</v>
       </c>
@@ -2845,7 +2861,7 @@
         <v>7025.1886666666669</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>1118803</v>
       </c>
@@ -2864,7 +2880,7 @@
         <v>35125.953333333331</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D96" t="s">
         <v>27</v>
       </c>
@@ -2873,7 +2889,7 @@
         <v>2600731.3900000006</v>
       </c>
     </row>
-    <row r="97" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C97" t="s">
         <v>24</v>
       </c>
@@ -2882,36 +2898,36 @@
       </c>
       <c r="G97" s="8"/>
     </row>
-    <row r="98" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:22" x14ac:dyDescent="0.3">
       <c r="E98" s="6"/>
       <c r="G98" s="8"/>
     </row>
-    <row r="99" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>80</v>
       </c>
       <c r="E99" s="6"/>
       <c r="G99" s="8"/>
     </row>
-    <row r="100" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>63</v>
       </c>
       <c r="E100" s="6"/>
       <c r="G100" s="8"/>
     </row>
-    <row r="101" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>96</v>
       </c>
       <c r="E101" s="6"/>
       <c r="G101" s="8"/>
     </row>
-    <row r="102" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:22" x14ac:dyDescent="0.3">
       <c r="E102" s="6"/>
       <c r="G102" s="8"/>
     </row>
-    <row r="103" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>1</v>
       </c>
@@ -2979,7 +2995,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="104" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>20</v>
       </c>
@@ -3030,7 +3046,7 @@
         <v>37286.400000000001</v>
       </c>
     </row>
-    <row r="105" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>20</v>
       </c>
@@ -3081,7 +3097,7 @@
         <v>4510.45</v>
       </c>
     </row>
-    <row r="106" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>20</v>
       </c>
@@ -3132,7 +3148,7 @@
         <v>135313.54999999999</v>
       </c>
     </row>
-    <row r="107" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>20</v>
       </c>
@@ -3183,7 +3199,7 @@
         <v>93216</v>
       </c>
     </row>
-    <row r="108" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>20</v>
       </c>
@@ -3234,7 +3250,7 @@
         <v>9321.6</v>
       </c>
     </row>
-    <row r="109" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A109" s="18" t="s">
         <v>20</v>
       </c>
@@ -3247,7 +3263,7 @@
       <c r="D109" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="E109" s="27">
+      <c r="E109" s="23">
         <v>43896</v>
       </c>
       <c r="F109" s="18">
@@ -3290,7 +3306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A110" s="18" t="s">
         <v>20</v>
       </c>
@@ -3303,7 +3319,7 @@
       <c r="D110" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="E110" s="27">
+      <c r="E110" s="23">
         <v>43896</v>
       </c>
       <c r="F110" s="18">
@@ -3346,15 +3362,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:22" x14ac:dyDescent="0.3">
       <c r="E111" s="6"/>
       <c r="G111" s="8"/>
     </row>
-    <row r="112" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:22" x14ac:dyDescent="0.3">
       <c r="E112" s="6"/>
       <c r="G112" s="8"/>
     </row>
-    <row r="113" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>70</v>
       </c>
@@ -3365,7 +3381,7 @@
       <c r="E113" s="6"/>
       <c r="G113" s="8"/>
     </row>
-    <row r="114" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>52</v>
       </c>
@@ -3378,7 +3394,7 @@
       <c r="E114" s="6"/>
       <c r="G114" s="8"/>
     </row>
-    <row r="115" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>1115230</v>
       </c>
@@ -3389,13 +3405,13 @@
         <f>B115/$B$120*$C$113</f>
         <v>1450.0266666666666</v>
       </c>
-      <c r="E115" s="23" t="s">
+      <c r="E115" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="F115" s="24"/>
+      <c r="F115" s="26"/>
       <c r="G115" s="8"/>
     </row>
-    <row r="116" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>1115231</v>
       </c>
@@ -3406,11 +3422,11 @@
         <f t="shared" ref="C116:C119" si="11">B116/$B$120*$C$113</f>
         <v>175.40646330666669</v>
       </c>
-      <c r="E116" s="24"/>
-      <c r="F116" s="24"/>
+      <c r="E116" s="26"/>
+      <c r="F116" s="26"/>
       <c r="G116" s="8"/>
     </row>
-    <row r="117" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>1115402</v>
       </c>
@@ -3424,7 +3440,7 @@
       <c r="E117" s="6"/>
       <c r="G117" s="8"/>
     </row>
-    <row r="118" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>1115403</v>
       </c>
@@ -3438,7 +3454,7 @@
       <c r="E118" s="6"/>
       <c r="G118" s="8"/>
     </row>
-    <row r="119" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>1115431</v>
       </c>
@@ -3452,7 +3468,7 @@
       <c r="E119" s="6"/>
       <c r="G119" s="8"/>
     </row>
-    <row r="120" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>81</v>
       </c>
@@ -3463,40 +3479,40 @@
       <c r="E120" s="6"/>
       <c r="G120" s="8"/>
     </row>
-    <row r="121" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:22" x14ac:dyDescent="0.3">
       <c r="E121" s="6"/>
       <c r="G121" s="8"/>
     </row>
-    <row r="122" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:22" x14ac:dyDescent="0.3">
       <c r="E122" s="6"/>
       <c r="G122" s="8"/>
     </row>
-    <row r="123" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>66</v>
       </c>
       <c r="E123" s="6"/>
       <c r="G123" s="8"/>
     </row>
-    <row r="124" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>63</v>
       </c>
       <c r="E124" s="6"/>
       <c r="G124" s="8"/>
     </row>
-    <row r="125" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>73</v>
       </c>
       <c r="E125" s="6"/>
       <c r="G125" s="8"/>
     </row>
-    <row r="126" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:22" x14ac:dyDescent="0.3">
       <c r="E126" s="6"/>
       <c r="G126" s="8"/>
     </row>
-    <row r="127" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>1</v>
       </c>
@@ -3564,7 +3580,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="128" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>20</v>
       </c>
@@ -3615,7 +3631,7 @@
         <v>725849.28</v>
       </c>
     </row>
-    <row r="129" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>20</v>
       </c>
@@ -3666,7 +3682,7 @@
         <v>18146.23</v>
       </c>
     </row>
-    <row r="130" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>20</v>
       </c>
@@ -3717,7 +3733,7 @@
         <v>18146.23</v>
       </c>
     </row>
-    <row r="131" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>20</v>
       </c>
@@ -3768,7 +3784,7 @@
         <v>18146.23</v>
       </c>
     </row>
-    <row r="132" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>20</v>
       </c>
@@ -3819,7 +3835,7 @@
         <v>18146.23</v>
       </c>
     </row>
-    <row r="133" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>20</v>
       </c>
@@ -3870,7 +3886,7 @@
         <v>18146.23</v>
       </c>
     </row>
-    <row r="134" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>20</v>
       </c>
@@ -3921,7 +3937,7 @@
         <v>90731.16</v>
       </c>
     </row>
-    <row r="135" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A135" s="12" t="s">
         <v>20</v>
       </c>
@@ -3978,11 +3994,11 @@
       </c>
       <c r="W135" s="12"/>
     </row>
-    <row r="136" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:23" x14ac:dyDescent="0.3">
       <c r="E136" s="6"/>
       <c r="G136" s="8"/>
     </row>
-    <row r="137" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>70</v>
       </c>
@@ -3996,7 +4012,7 @@
       <c r="E137" s="6"/>
       <c r="G137" s="8"/>
     </row>
-    <row r="138" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>52</v>
       </c>
@@ -4009,7 +4025,7 @@
       <c r="E138" s="6"/>
       <c r="G138" s="8"/>
     </row>
-    <row r="139" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>1115403</v>
       </c>
@@ -4021,13 +4037,13 @@
         <f>B139/$B$146*$C$137</f>
         <v>80649.919999999998</v>
       </c>
-      <c r="E139" s="23" t="s">
+      <c r="E139" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="F139" s="24"/>
+      <c r="F139" s="26"/>
       <c r="G139" s="8"/>
     </row>
-    <row r="140" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>1118798</v>
       </c>
@@ -4039,11 +4055,11 @@
         <f t="shared" ref="C140:C145" si="13">B140/$B$146*$C$137</f>
         <v>2016.2479999999998</v>
       </c>
-      <c r="E140" s="24"/>
-      <c r="F140" s="24"/>
+      <c r="E140" s="26"/>
+      <c r="F140" s="26"/>
       <c r="G140" s="8"/>
     </row>
-    <row r="141" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>1118799</v>
       </c>
@@ -4058,7 +4074,7 @@
       <c r="E141" s="6"/>
       <c r="G141" s="8"/>
     </row>
-    <row r="142" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>1118800</v>
       </c>
@@ -4073,7 +4089,7 @@
       <c r="E142" s="6"/>
       <c r="G142" s="8"/>
     </row>
-    <row r="143" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>1118801</v>
       </c>
@@ -4088,7 +4104,7 @@
       <c r="E143" s="6"/>
       <c r="G143" s="8"/>
     </row>
-    <row r="144" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>1118802</v>
       </c>
@@ -4103,7 +4119,7 @@
       <c r="E144" s="6"/>
       <c r="G144" s="8"/>
     </row>
-    <row r="145" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>1118803</v>
       </c>
@@ -4118,7 +4134,7 @@
       <c r="E145" s="6"/>
       <c r="G145" s="8"/>
     </row>
-    <row r="146" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>53</v>
       </c>
@@ -4129,47 +4145,47 @@
       <c r="E146" s="6"/>
       <c r="G146" s="8"/>
     </row>
-    <row r="147" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:22" x14ac:dyDescent="0.3">
       <c r="E147" s="6"/>
       <c r="G147" s="8"/>
     </row>
-    <row r="148" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:22" x14ac:dyDescent="0.3">
       <c r="E148" s="6"/>
       <c r="G148" s="8"/>
     </row>
-    <row r="149" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>72</v>
       </c>
       <c r="E149" s="6"/>
       <c r="G149" s="8"/>
     </row>
-    <row r="150" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>63</v>
       </c>
       <c r="E150" s="6"/>
       <c r="G150" s="8"/>
     </row>
-    <row r="151" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>95</v>
       </c>
       <c r="E151" s="6"/>
       <c r="G151" s="8"/>
     </row>
-    <row r="152" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:22" x14ac:dyDescent="0.3">
       <c r="E152" s="6"/>
       <c r="G152" s="8"/>
     </row>
-    <row r="153" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>76</v>
       </c>
       <c r="E153" s="6"/>
       <c r="G153" s="8"/>
     </row>
-    <row r="154" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>1</v>
       </c>
@@ -4237,7 +4253,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="155" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A155" s="5" t="s">
         <v>20</v>
       </c>
@@ -4250,7 +4266,7 @@
       <c r="D155" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E155" s="28">
+      <c r="E155" s="24">
         <v>43921</v>
       </c>
       <c r="F155" s="5">
@@ -4293,7 +4309,7 @@
         <v>334981.44</v>
       </c>
     </row>
-    <row r="156" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A156" s="5" t="s">
         <v>20</v>
       </c>
@@ -4306,7 +4322,7 @@
       <c r="D156" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E156" s="28">
+      <c r="E156" s="24">
         <v>43921</v>
       </c>
       <c r="F156" s="5">
@@ -4349,7 +4365,7 @@
         <v>40521.949999999997</v>
       </c>
     </row>
-    <row r="157" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A157" s="5" t="s">
         <v>20</v>
       </c>
@@ -4362,7 +4378,7 @@
       <c r="D157" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E157" s="28">
+      <c r="E157" s="24">
         <v>43921</v>
       </c>
       <c r="F157" s="5">
@@ -4405,7 +4421,7 @@
         <v>1215658.45</v>
       </c>
     </row>
-    <row r="158" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A158" s="5" t="s">
         <v>20</v>
       </c>
@@ -4418,7 +4434,7 @@
       <c r="D158" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E158" s="28">
+      <c r="E158" s="24">
         <v>43921</v>
       </c>
       <c r="F158" s="5">
@@ -4461,7 +4477,7 @@
         <v>669962.88</v>
       </c>
     </row>
-    <row r="159" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A159" s="5" t="s">
         <v>20</v>
       </c>
@@ -4474,7 +4490,7 @@
       <c r="D159" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E159" s="28">
+      <c r="E159" s="24">
         <v>43921</v>
       </c>
       <c r="F159" s="5">
@@ -4517,7 +4533,7 @@
         <v>83745.36</v>
       </c>
     </row>
-    <row r="160" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>20</v>
       </c>
@@ -4568,7 +4584,7 @@
         <v>16749.07</v>
       </c>
     </row>
-    <row r="161" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>20</v>
       </c>
@@ -4619,7 +4635,7 @@
         <v>16749.07</v>
       </c>
     </row>
-    <row r="162" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>20</v>
       </c>
@@ -4670,7 +4686,7 @@
         <v>16749.07</v>
       </c>
     </row>
-    <row r="163" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>20</v>
       </c>
@@ -4721,7 +4737,7 @@
         <v>16749.07</v>
       </c>
     </row>
-    <row r="164" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>20</v>
       </c>
@@ -4772,7 +4788,7 @@
         <v>16749.07</v>
       </c>
     </row>
-    <row r="165" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>20</v>
       </c>
@@ -4823,7 +4839,7 @@
         <v>83745.36</v>
       </c>
     </row>
-    <row r="166" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A166" s="12" t="s">
         <v>20</v>
       </c>
@@ -4879,11 +4895,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:22" x14ac:dyDescent="0.3">
       <c r="E167" s="6"/>
       <c r="G167" s="8"/>
     </row>
-    <row r="168" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>70</v>
       </c>
@@ -4896,7 +4912,7 @@
       </c>
       <c r="E168" s="6"/>
     </row>
-    <row r="169" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>52</v>
       </c>
@@ -4908,7 +4924,7 @@
       </c>
       <c r="E169" s="6"/>
     </row>
-    <row r="170" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A170" s="5">
         <v>1115230</v>
       </c>
@@ -4920,12 +4936,12 @@
         <f>B170/$B$181*$C$168</f>
         <v>13440.613333333335</v>
       </c>
-      <c r="E170" s="23" t="s">
+      <c r="E170" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="F170" s="24"/>
-    </row>
-    <row r="171" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F170" s="26"/>
+    </row>
+    <row r="171" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A171" s="5">
         <v>1115231</v>
       </c>
@@ -4937,10 +4953,10 @@
         <f t="shared" ref="C171:C180" si="15">B171/$B$181*$C$168</f>
         <v>1625.8807535533335</v>
       </c>
-      <c r="E171" s="24"/>
-      <c r="F171" s="24"/>
-    </row>
-    <row r="172" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E171" s="26"/>
+      <c r="F171" s="26"/>
+    </row>
+    <row r="172" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A172" s="5">
         <v>1115402</v>
       </c>
@@ -4954,7 +4970,7 @@
       </c>
       <c r="E172" s="6"/>
     </row>
-    <row r="173" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A173" s="5">
         <v>1115403</v>
       </c>
@@ -4968,7 +4984,7 @@
       </c>
       <c r="E173" s="6"/>
     </row>
-    <row r="174" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A174" s="5">
         <v>1115431</v>
       </c>
@@ -4982,7 +4998,7 @@
       </c>
       <c r="E174" s="6"/>
     </row>
-    <row r="175" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>1118798</v>
       </c>
@@ -4996,7 +5012,7 @@
       </c>
       <c r="E175" s="6"/>
     </row>
-    <row r="176" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>1118799</v>
       </c>
@@ -5010,7 +5026,7 @@
       </c>
       <c r="E176" s="6"/>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>1118800</v>
       </c>
@@ -5024,7 +5040,7 @@
       </c>
       <c r="E177" s="6"/>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>1118801</v>
       </c>
@@ -5038,7 +5054,7 @@
       </c>
       <c r="E178" s="6"/>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>1118802</v>
       </c>
@@ -5052,7 +5068,7 @@
       </c>
       <c r="E179" s="6"/>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>1118803</v>
       </c>
@@ -5066,7 +5082,7 @@
       </c>
       <c r="E180" s="6"/>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>81</v>
       </c>
@@ -5076,23 +5092,23 @@
       </c>
       <c r="E181" s="6"/>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E182" s="6"/>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B184" s="25" t="s">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B184" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="C184" s="26"/>
-      <c r="D184" s="26"/>
-      <c r="E184" s="26"/>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C184" s="28"/>
+      <c r="D184" s="28"/>
+      <c r="E184" s="28"/>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>52</v>
       </c>
@@ -5106,10 +5122,10 @@
         <v>88</v>
       </c>
       <c r="E185" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" s="5">
         <v>1115230</v>
       </c>
@@ -5125,7 +5141,7 @@
         <v>14890.640000000001</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" s="5">
         <v>1115231</v>
       </c>
@@ -5141,7 +5157,7 @@
         <v>1801.2872168600002</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" s="5">
         <v>1115402</v>
       </c>
@@ -5157,7 +5173,7 @@
         <v>54038.612783140001</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" s="5">
         <v>1115403</v>
       </c>
@@ -5175,7 +5191,7 @@
         <v>111156.21333333333</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" s="5">
         <v>1115431</v>
       </c>
@@ -5191,7 +5207,7 @@
         <v>3722.6600000000003</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>1118798</v>
       </c>
@@ -5207,7 +5223,7 @@
         <v>2688.2786666666666</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>1118799</v>
       </c>
@@ -5223,7 +5239,7 @@
         <v>2688.2786666666666</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>1118800</v>
       </c>
@@ -5239,7 +5255,7 @@
         <v>2688.2786666666666</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>1118801</v>
       </c>
@@ -5255,7 +5271,7 @@
         <v>2688.2786666666666</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>1118802</v>
       </c>
@@ -5271,7 +5287,7 @@
         <v>2688.2786666666666</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>1118803</v>
       </c>
@@ -5287,13 +5303,13 @@
         <v>13441.393333333333</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E197" s="6"/>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E198" s="6"/>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A199" s="3" t="s">
         <v>90</v>
       </c>
@@ -5304,7 +5320,7 @@
       </c>
       <c r="E199" s="6"/>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>25</v>
       </c>
@@ -5324,7 +5340,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>1005742</v>
       </c>
@@ -5348,7 +5364,7 @@
         <v>43935</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>1005743</v>
       </c>
@@ -5372,7 +5388,7 @@
         <v>43937</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>1005744</v>
       </c>
@@ -5396,7 +5412,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>1005745</v>
       </c>
@@ -5423,7 +5439,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>1005746</v>
       </c>
@@ -5453,7 +5469,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>1005747</v>
       </c>
@@ -5483,7 +5499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>1005748</v>
       </c>
@@ -5507,7 +5523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>1005749</v>
       </c>
@@ -5525,7 +5541,7 @@
         <v>17854.940000000002</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>1005750</v>
       </c>
@@ -5546,7 +5562,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>1005751</v>
       </c>
@@ -5567,7 +5583,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>1005752</v>
       </c>
@@ -5588,7 +5604,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>1005753</v>
       </c>
@@ -5609,7 +5625,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A213" s="4">
         <v>1005791</v>
       </c>
@@ -5627,7 +5643,7 @@
         <v>17696.159999999974</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A214" s="4">
         <v>1005793</v>
       </c>
@@ -5648,7 +5664,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>1005841</v>
       </c>
@@ -5669,7 +5685,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>1005842</v>
       </c>
@@ -5687,7 +5703,7 @@
         <v>2749.66</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>1005843</v>
       </c>
@@ -5705,7 +5721,7 @@
         <v>1392.6800000000003</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>1005844</v>
       </c>
@@ -5723,7 +5739,7 @@
         <v>7141.9800000000032</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>1007914</v>
       </c>
@@ -5741,7 +5757,7 @@
         <v>64277.820000000007</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>1007921</v>
       </c>
@@ -5759,7 +5775,7 @@
         <v>321389.07000000007</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>1007922</v>
       </c>
@@ -5777,7 +5793,7 @@
         <v>160694.53000000003</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>1007923</v>
       </c>
@@ -5795,7 +5811,7 @@
         <v>107129.68999999994</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>1007924</v>
       </c>
@@ -5813,7 +5829,7 @@
         <v>40709.279999999999</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>1007925</v>
       </c>
@@ -5831,7 +5847,7 @@
         <v>160694.53000000003</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>1007926</v>
       </c>
@@ -5849,7 +5865,7 @@
         <v>128555.62</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>1007928</v>
       </c>
@@ -5867,7 +5883,7 @@
         <v>160694.53000000003</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>1007929</v>
       </c>
@@ -5885,7 +5901,7 @@
         <v>160694.53000000003</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>1007930</v>
       </c>
@@ -5903,7 +5919,7 @@
         <v>321389.07000000007</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>1007935</v>
       </c>
@@ -5921,7 +5937,7 @@
         <v>160694.53000000003</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>1007937</v>
       </c>
@@ -5939,7 +5955,7 @@
         <v>64277.820000000007</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>1008407</v>
       </c>
@@ -5957,7 +5973,7 @@
         <v>321389.07000000007</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>1008480</v>
       </c>
@@ -5975,7 +5991,7 @@
         <v>6749.1700000000019</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>1008482</v>
       </c>
@@ -5993,7 +6009,7 @@
         <v>18390.599999999991</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>1008484</v>
       </c>
@@ -6011,7 +6027,7 @@
         <v>9177.4399999999951</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>1017308</v>
       </c>
@@ -6029,7 +6045,7 @@
         <v>14283.949999999997</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D236" t="s">
         <v>0</v>
       </c>
@@ -6038,7 +6054,7 @@
         <v>2581301.2300000004</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C237" t="s">
         <v>24</v>
       </c>
@@ -6046,22 +6062,22 @@
         <v>2581301.23</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="241" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="243" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>2</v>
       </c>
@@ -6126,7 +6142,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="244" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>45</v>
       </c>
@@ -6173,7 +6189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>45</v>
       </c>
@@ -6220,7 +6236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A246" s="12" t="s">
         <v>45</v>
       </c>
@@ -6273,7 +6289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>70</v>
       </c>
@@ -6285,7 +6301,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="249" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>52</v>
       </c>
@@ -6296,7 +6312,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="250" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>1005791</v>
       </c>
@@ -6308,7 +6324,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="251" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>1005793</v>
       </c>
@@ -6320,7 +6336,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="252" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>53</v>
       </c>
@@ -6329,474 +6345,484 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A254" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="256" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A256" s="22" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A257" t="s">
+    <row r="254" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A254" s="29" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="255" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A255" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A257" s="22" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A258" t="s">
         <v>70</v>
       </c>
-      <c r="C257" s="6">
+      <c r="C258" s="6">
         <f>T246</f>
         <v>1108407.3</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A258" t="s">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A259" t="s">
         <v>52</v>
       </c>
-      <c r="B258" t="s">
+      <c r="B259" t="s">
         <v>26</v>
       </c>
-      <c r="C258" t="s">
+      <c r="C259" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A259">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A260">
         <v>1005791</v>
       </c>
-      <c r="B259">
+      <c r="B260">
         <f>J252</f>
         <v>0</v>
       </c>
-      <c r="C259" s="20">
+      <c r="C260" s="20">
         <f>T244</f>
         <v>-184734.55</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A260">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A261">
         <v>1005793</v>
       </c>
-      <c r="B260">
-        <f>J253</f>
-        <v>0</v>
-      </c>
-      <c r="C260" s="20">
+      <c r="B261">
+        <f>J254</f>
+        <v>0</v>
+      </c>
+      <c r="C261" s="20">
         <f>T245</f>
         <v>-923672.75</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A262" t="s">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A263" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A263" t="s">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A264" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A265" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A266" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A268" s="22" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A264" t="s">
+    <row r="269" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A269" t="s">
+        <v>70</v>
+      </c>
+      <c r="C269" s="6">
+        <f>C258+C260</f>
+        <v>923672.75</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A270" t="s">
+        <v>52</v>
+      </c>
+      <c r="B270" t="s">
+        <v>26</v>
+      </c>
+      <c r="C270" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A271">
+        <v>1005793</v>
+      </c>
+      <c r="B271">
+        <f>J265</f>
+        <v>0</v>
+      </c>
+      <c r="C271" s="20">
+        <f>C261</f>
+        <v>-923672.75</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A273" s="22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A274" t="s">
+        <v>70</v>
+      </c>
+      <c r="C274" s="6">
+        <f>C263+C265</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A275" t="s">
+        <v>52</v>
+      </c>
+      <c r="B275" t="s">
+        <v>26</v>
+      </c>
+      <c r="C275" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C276" s="20"/>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A277" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A278" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A280" t="s">
+        <v>70</v>
+      </c>
+      <c r="C280" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A281" t="s">
+        <v>52</v>
+      </c>
+      <c r="B281" t="s">
+        <v>26</v>
+      </c>
+      <c r="C281" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A282" t="s">
+        <v>105</v>
+      </c>
+      <c r="B282" t="s">
+        <v>108</v>
+      </c>
+      <c r="C282" s="20" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A283" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A266" s="22" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A267" t="s">
-        <v>70</v>
-      </c>
-      <c r="C267" s="6">
-        <f>C257+C259</f>
-        <v>923672.75</v>
-      </c>
-    </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A268" t="s">
-        <v>52</v>
-      </c>
-      <c r="B268" t="s">
-        <v>26</v>
-      </c>
-      <c r="C268" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A269">
-        <v>1005793</v>
-      </c>
-      <c r="B269">
-        <f>J264</f>
-        <v>0</v>
-      </c>
-      <c r="C269" s="20">
-        <f>C260</f>
-        <v>-923672.75</v>
-      </c>
-    </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A271" s="22" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A272" t="s">
-        <v>70</v>
-      </c>
-      <c r="C272" s="6">
-        <f>C262+C264</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A273" t="s">
-        <v>52</v>
-      </c>
-      <c r="B273" t="s">
-        <v>26</v>
-      </c>
-      <c r="C273" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C274" s="20"/>
-    </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A275" t="s">
+      <c r="B283" t="s">
+        <v>109</v>
+      </c>
+      <c r="C283" s="20" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A284" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A276" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A278" t="s">
-        <v>70</v>
-      </c>
-      <c r="C278" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A279" t="s">
-        <v>52</v>
-      </c>
-      <c r="B279" t="s">
-        <v>26</v>
-      </c>
-      <c r="C279" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A280" t="s">
-        <v>108</v>
-      </c>
-      <c r="B280" t="s">
-        <v>111</v>
-      </c>
-      <c r="C280" s="20" t="s">
+      <c r="B284" t="s">
+        <v>110</v>
+      </c>
+      <c r="C284" s="20" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A281" t="s">
-        <v>109</v>
-      </c>
-      <c r="B281" t="s">
-        <v>112</v>
-      </c>
-      <c r="C281" s="20" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A282" t="s">
-        <v>110</v>
-      </c>
-      <c r="B282" t="s">
+    <row r="285" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A285" t="s">
+        <v>81</v>
+      </c>
+      <c r="B285" t="s">
         <v>113</v>
       </c>
-      <c r="C282" s="20" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A283" t="s">
-        <v>81</v>
-      </c>
-      <c r="B283" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A286" s="3" t="s">
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A288" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B286" s="3"/>
-      <c r="C286" s="3"/>
-      <c r="D286" s="3" t="s">
+      <c r="B288" s="3"/>
+      <c r="C288" s="3"/>
+      <c r="D288" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A287" t="s">
+    <row r="289" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A289" t="s">
         <v>25</v>
       </c>
-      <c r="B287" t="s">
+      <c r="B289" t="s">
         <v>28</v>
       </c>
-      <c r="C287" t="s">
+      <c r="C289" t="s">
         <v>29</v>
       </c>
-      <c r="D287" t="s">
+      <c r="D289" t="s">
         <v>69</v>
       </c>
-      <c r="E287" t="s">
-        <v>0</v>
-      </c>
-      <c r="F287" t="s">
+      <c r="E289" t="s">
+        <v>0</v>
+      </c>
+      <c r="F289" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A288">
+    <row r="290" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A290">
         <v>1108340</v>
       </c>
-      <c r="B288" s="6">
+      <c r="B290" s="6">
         <v>679093.73</v>
       </c>
-      <c r="C288" s="6">
+      <c r="C290" s="6">
         <v>726198.49</v>
       </c>
-      <c r="D288" s="6">
-        <v>0</v>
-      </c>
-      <c r="E288" s="8">
-        <f>C288-B288+D288</f>
+      <c r="D290" s="6">
+        <v>0</v>
+      </c>
+      <c r="E290" s="8">
+        <f>C290-B290+D290</f>
         <v>47104.760000000009</v>
       </c>
-      <c r="F288" s="6">
+      <c r="F290" s="6">
         <v>47104.76</v>
       </c>
     </row>
-    <row r="289" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B289" s="6"/>
-      <c r="C289" s="6"/>
-      <c r="D289" s="8"/>
-      <c r="E289" s="6"/>
-    </row>
-    <row r="290" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A290" t="s">
-        <v>55</v>
-      </c>
-      <c r="B290" s="6"/>
-      <c r="C290" s="6"/>
-      <c r="D290" s="8"/>
-      <c r="E290" s="6"/>
-    </row>
-    <row r="291" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A291" t="s">
-        <v>56</v>
-      </c>
+    <row r="291" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B291" s="6"/>
       <c r="C291" s="6"/>
       <c r="D291" s="8"/>
       <c r="E291" s="6"/>
     </row>
-    <row r="292" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B292" s="6"/>
       <c r="C292" s="6"/>
       <c r="D292" s="8"/>
       <c r="E292" s="6"/>
     </row>
-    <row r="293" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
+        <v>56</v>
+      </c>
+      <c r="B293" s="6"/>
+      <c r="C293" s="6"/>
+      <c r="D293" s="8"/>
+      <c r="E293" s="6"/>
+    </row>
+    <row r="294" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A294" t="s">
+        <v>57</v>
+      </c>
+      <c r="B294" s="6"/>
+      <c r="C294" s="6"/>
+      <c r="D294" s="8"/>
+      <c r="E294" s="6"/>
+    </row>
+    <row r="295" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A295" t="s">
         <v>1</v>
       </c>
-      <c r="B293" s="6" t="s">
+      <c r="B295" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C293" s="6" t="s">
+      <c r="C295" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D293" s="8" t="s">
+      <c r="D295" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E293" s="6" t="s">
+      <c r="E295" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F293" t="s">
+      <c r="F295" t="s">
         <v>6</v>
       </c>
-      <c r="G293" t="s">
+      <c r="G295" t="s">
         <v>7</v>
       </c>
-      <c r="H293" t="s">
+      <c r="H295" t="s">
         <v>8</v>
       </c>
-      <c r="I293" t="s">
+      <c r="I295" t="s">
         <v>9</v>
       </c>
-      <c r="J293" t="s">
+      <c r="J295" t="s">
         <v>10</v>
       </c>
-      <c r="K293" t="s">
+      <c r="K295" t="s">
         <v>11</v>
       </c>
-      <c r="L293" t="s">
+      <c r="L295" t="s">
         <v>12</v>
       </c>
-      <c r="M293" t="s">
+      <c r="M295" t="s">
         <v>42</v>
       </c>
-      <c r="N293" t="s">
+      <c r="N295" t="s">
         <v>43</v>
       </c>
-      <c r="O293" t="s">
+      <c r="O295" t="s">
         <v>44</v>
       </c>
-      <c r="P293" t="s">
+      <c r="P295" t="s">
         <v>13</v>
       </c>
-      <c r="Q293" t="s">
+      <c r="Q295" t="s">
         <v>14</v>
       </c>
-      <c r="R293" t="s">
+      <c r="R295" t="s">
         <v>15</v>
       </c>
-      <c r="S293" t="s">
+      <c r="S295" t="s">
         <v>16</v>
       </c>
-      <c r="T293" t="s">
+      <c r="T295" t="s">
         <v>17</v>
       </c>
-      <c r="U293" t="s">
+      <c r="U295" t="s">
         <v>18</v>
       </c>
-      <c r="V293" t="s">
+      <c r="V295" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="294" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A294" s="12" t="s">
+    <row r="296" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A296" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B294" s="14" t="s">
+      <c r="B296" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C294" s="14" t="s">
+      <c r="C296" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D294" s="15" t="s">
+      <c r="D296" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="E294" s="16">
+      <c r="E296" s="16">
         <v>43843</v>
       </c>
-      <c r="F294" s="12">
-        <v>0</v>
-      </c>
-      <c r="G294" s="12"/>
-      <c r="H294" s="12">
+      <c r="F296" s="12">
+        <v>0</v>
+      </c>
+      <c r="G296" s="12"/>
+      <c r="H296" s="12">
         <v>1108338</v>
       </c>
-      <c r="I294" s="12">
-        <v>0</v>
-      </c>
-      <c r="J294" s="12"/>
-      <c r="K294" s="12">
-        <v>0</v>
-      </c>
-      <c r="L294" s="12"/>
-      <c r="M294" s="12"/>
-      <c r="N294" s="12"/>
-      <c r="O294" s="12"/>
-      <c r="P294" s="14">
+      <c r="I296" s="12">
+        <v>0</v>
+      </c>
+      <c r="J296" s="12"/>
+      <c r="K296" s="12">
+        <v>0</v>
+      </c>
+      <c r="L296" s="12"/>
+      <c r="M296" s="12"/>
+      <c r="N296" s="12"/>
+      <c r="O296" s="12"/>
+      <c r="P296" s="14">
         <v>726198.49</v>
       </c>
-      <c r="Q294" s="14">
-        <v>0</v>
-      </c>
-      <c r="R294" s="14">
-        <v>0</v>
-      </c>
-      <c r="S294" s="14">
+      <c r="Q296" s="14">
+        <v>0</v>
+      </c>
+      <c r="R296" s="14">
+        <v>0</v>
+      </c>
+      <c r="S296" s="14">
         <v>726198.49</v>
       </c>
-      <c r="T294" s="14">
-        <v>0</v>
-      </c>
-      <c r="U294" s="14">
+      <c r="T296" s="14">
+        <v>0</v>
+      </c>
+      <c r="U296" s="14">
         <v>726198.49</v>
       </c>
-      <c r="V294" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="295" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A295" t="s">
+      <c r="V296" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="297" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A297" t="s">
         <v>20</v>
       </c>
-      <c r="B295" s="6" t="s">
+      <c r="B297" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C295" s="6" t="s">
+      <c r="C297" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D295" s="8" t="s">
+      <c r="D297" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E295" s="11">
+      <c r="E297" s="11">
         <v>43843</v>
       </c>
-      <c r="F295">
-        <v>0</v>
-      </c>
-      <c r="H295">
+      <c r="F297">
+        <v>0</v>
+      </c>
+      <c r="H297">
         <v>1108340</v>
       </c>
-      <c r="I295">
-        <v>0</v>
-      </c>
-      <c r="K295">
-        <v>0</v>
-      </c>
-      <c r="P295" s="6">
+      <c r="I297">
+        <v>0</v>
+      </c>
+      <c r="K297">
+        <v>0</v>
+      </c>
+      <c r="P297" s="6">
         <v>-726198.49</v>
       </c>
-      <c r="Q295" s="6">
+      <c r="Q297" s="6">
         <v>726198.49</v>
       </c>
-      <c r="R295" s="6">
+      <c r="R297" s="6">
         <v>-726198.49</v>
       </c>
-      <c r="S295" s="6">
-        <v>0</v>
-      </c>
-      <c r="T295" s="6">
-        <v>0</v>
-      </c>
-      <c r="U295" s="6">
+      <c r="S297" s="6">
+        <v>0</v>
+      </c>
+      <c r="T297" s="6">
+        <v>0</v>
+      </c>
+      <c r="U297" s="6">
         <v>-726198.49</v>
       </c>
-      <c r="V295">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="297" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A297" t="s">
-        <v>120</v>
+      <c r="V297">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A299" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -6815,6 +6841,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A3ABBA213F535143A2153FAFFCD4B404" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="00705d5726f6d16a2d41866951f40978">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="56ce6572-a240-4cd6-8225-c99230995deb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="da66d2f5d03ddcf0575955673b1bb8c9" ns2:_="">
     <xsd:import namespace="56ce6572-a240-4cd6-8225-c99230995deb"/>
@@ -6992,22 +7033,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86950AF1-3B0F-4325-898D-5495113D013F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9D5D619-8B2D-4F02-88F7-AF4B83361BA6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6CF752EA-8C3D-49D6-BA76-CD10A9A117BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7023,21 +7066,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9D5D619-8B2D-4F02-88F7-AF4B83361BA6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86950AF1-3B0F-4325-898D-5495113D013F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>